<commit_message>
Added new Servants released on JP summer 2020
- Sessyoin Kiara
- Ilyasviel
- Brynhildr
- Murasaki
- Tomoe Gozen
- Abigail Williams
</commit_message>
<xml_diff>
--- a/Total Servant Database.xlsx
+++ b/Total Servant Database.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH281"/>
+  <dimension ref="A1:AH287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>Divine, Greek Mythology Males, Humanoid, King, Male, Riding, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Divine, Greek Mythology Males, Humanoid, King, Male, Riding, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
@@ -5266,7 +5266,7 @@
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>Humanoid, Male, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Humanoid, Male, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
@@ -8156,7 +8156,7 @@
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>Giant, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Giant, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
@@ -8592,7 +8592,7 @@
       </c>
       <c r="Y57" t="inlineStr">
         <is>
-          <t>Dragon, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Dragon, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z57" t="inlineStr">
@@ -11190,7 +11190,7 @@
       </c>
       <c r="Y75" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants (Stage2-3), Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z75" t="inlineStr">
@@ -11334,7 +11334,7 @@
       </c>
       <c r="Y76" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z76" t="inlineStr">
@@ -14219,7 +14219,7 @@
       </c>
       <c r="Y96" t="inlineStr">
         <is>
-          <t>Divine, Humanoid, King, Male, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Divine, Humanoid, King, Male, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z96" t="inlineStr">
@@ -17393,7 +17393,7 @@
       </c>
       <c r="Y118" t="inlineStr">
         <is>
-          <t>Demonic, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Demonic, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z118" t="inlineStr">
@@ -19985,7 +19985,7 @@
       </c>
       <c r="Y136" t="inlineStr">
         <is>
-          <t>Dragon, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Dragon, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z136" t="inlineStr">
@@ -20273,7 +20273,7 @@
       </c>
       <c r="Y138" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Illya, Living Human, Pseudo-Servants, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Illya, Living Human, Pseudo-Servants, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z138" t="inlineStr">
@@ -20417,7 +20417,7 @@
       </c>
       <c r="Y139" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Living Human, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Living Human, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z139" t="inlineStr">
@@ -20993,7 +20993,7 @@
       </c>
       <c r="Y143" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Saberface, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Saberface, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z143" t="inlineStr">
@@ -21713,7 +21713,7 @@
       </c>
       <c r="Y148" t="inlineStr">
         <is>
-          <t>Divine, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Divine, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z148" t="inlineStr">
@@ -23587,7 +23587,7 @@
       </c>
       <c r="Y161" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z161" t="inlineStr">
@@ -24595,7 +24595,7 @@
       </c>
       <c r="Y168" t="inlineStr">
         <is>
-          <t>Female, Humanoid, King, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, King, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z168" t="inlineStr">
@@ -25173,7 +25173,7 @@
       </c>
       <c r="Y172" t="inlineStr">
         <is>
-          <t>Female, Giant, Humanoid, Servants, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Giant, Humanoid, Servants, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z172" t="inlineStr">
@@ -28201,7 +28201,7 @@
       </c>
       <c r="Y193" t="inlineStr">
         <is>
-          <t>Divine, Female, Humanoid, Servant, Threat to Humanity</t>
+          <t>Children Servants, Divine, Female, Humanoid, Servant, Threat to Humanity</t>
         </is>
       </c>
       <c r="Z193" t="inlineStr">
@@ -30280,7 +30280,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Manslayer Izō (人斬り以蔵, Hitokiri Izō?), Okada Izou</t>
+          <t>Manslayer Izō (人斬り以蔵, Hitokiri Izō?), Okada Izou, Ghost of Tosa</t>
         </is>
       </c>
       <c r="G208" t="n">
@@ -31369,7 +31369,7 @@
       </c>
       <c r="Y215" t="inlineStr">
         <is>
-          <t>Demonic, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Demonic, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z215" t="inlineStr">
@@ -32377,7 +32377,7 @@
       </c>
       <c r="Y222" t="inlineStr">
         <is>
-          <t>Divine, Female, Humanoid, Illya, Pseudo-Servant, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Divine, Female, Humanoid, Illya, Pseudo-Servant, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z222" t="inlineStr">
@@ -33141,7 +33141,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Yu Miaoyi</t>
+          <t>Consort Yu</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -33164,7 +33164,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Consort Yu, Yu the Beauty, Yu Meiren, Akuta Hinako (芥ヒナコ?)Crimson Beauty Under the Moon (紅の月下美人?), Gubijin, Gucchan, 虞妙弋</t>
+          <t>Yu Miaoyi, Yu the Beauty, Yu Meiren, Akuta Hinako (芥ヒナコ?)Crimson Beauty Under the Moon (紅の月下美人?), Gubijin, Gucchan, 虞妙弋</t>
         </is>
       </c>
       <c r="G228" t="n">
@@ -33819,7 +33819,7 @@
       </c>
       <c r="Y232" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z232" t="inlineStr">
@@ -34107,7 +34107,7 @@
       </c>
       <c r="Y234" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Living Human, Pseudo-Servants, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Female, Humanoid, Living Human, Pseudo-Servants, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z234" t="inlineStr">
@@ -34541,7 +34541,7 @@
       </c>
       <c r="Y237" t="inlineStr">
         <is>
-          <t>Divine, Female, Humanoid, Pseudo-Servant, Riding, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants (Stage 1), Divine, Female, Humanoid, Pseudo-Servant, Riding, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z237" t="inlineStr">
@@ -35839,7 +35839,7 @@
       </c>
       <c r="Y246" t="inlineStr">
         <is>
-          <t>Argo-Related, Brynhildr's Beloved, Divine, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
+          <t>Argo-Related, Divine, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z246" t="inlineStr">
@@ -36338,7 +36338,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>Loli Vinci, Gran Cavallo</t>
+          <t>Da Vinci Lily, Loli Vinci, Gran Cavallo</t>
         </is>
       </c>
       <c r="G250" t="n">
@@ -36417,7 +36417,7 @@
       </c>
       <c r="Y250" t="inlineStr">
         <is>
-          <t>Female, Humanoid, Riding, Servant</t>
+          <t>Children Servants, Female, Humanoid, Riding, Servant</t>
         </is>
       </c>
       <c r="Z250" t="inlineStr">
@@ -36705,7 +36705,7 @@
       </c>
       <c r="Y252" t="inlineStr">
         <is>
-          <t>Argo-Related, Brynhildr's Beloved, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
+          <t>Argo-Related, Brynhildr's Beloved, Children Servants, Greek Mythology Males, Humanoid, Male, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z252" t="inlineStr">
@@ -39188,7 +39188,11 @@
           <t>Arts</t>
         </is>
       </c>
-      <c r="AH269" t="inlineStr"/>
+      <c r="AH269" t="inlineStr">
+        <is>
+          <t>－</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -40447,7 +40451,7 @@
       </c>
       <c r="Y278" t="inlineStr">
         <is>
-          <t>Humanoid, Male, Servant</t>
+          <t>Children Servants, Humanoid, Male, Servant</t>
         </is>
       </c>
       <c r="Z278" t="inlineStr">
@@ -40735,7 +40739,7 @@
       </c>
       <c r="Y280" t="inlineStr">
         <is>
-          <t>Divine, Female, Humanoid, Living Human, Riding, Servant, Weak to Enuma Elish</t>
+          <t>Children Servants, Divine, Female, Humanoid, Living Human, Riding, Servant, Weak to Enuma Elish</t>
         </is>
       </c>
       <c r="Z280" t="inlineStr">
@@ -40800,7 +40804,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Artoria Pendragon (Caster)</t>
+          <t>Castoria, CasSeiba</t>
         </is>
       </c>
       <c r="G281" t="n">
@@ -40879,7 +40883,7 @@
       </c>
       <c r="Y281" t="inlineStr">
         <is>
-          <t>Arthur, Humanoid, Saberface, Servant</t>
+          <t>Arthur, Humanoid, Saberface, Servant, Female</t>
         </is>
       </c>
       <c r="Z281" t="inlineStr">
@@ -40918,6 +40922,870 @@
         <is>
           <t>－</t>
         </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Sesshōin Kiara (Moon Cancer)</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>285</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>5-Star</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Moon Cancer</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>殺生院キアラ</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Sessyoin Kiara, Sesshouin Kiara, Demonic Bodhisattva, Last Prophet, Beast III/R</t>
+        </is>
+      </c>
+      <c r="G282" t="n">
+        <v>16</v>
+      </c>
+      <c r="H282" t="n">
+        <v>1719</v>
+      </c>
+      <c r="I282" t="n">
+        <v>11128</v>
+      </c>
+      <c r="J282" t="n">
+        <v>2249</v>
+      </c>
+      <c r="K282" t="n">
+        <v>15336</v>
+      </c>
+      <c r="L282" t="n">
+        <v>12181</v>
+      </c>
+      <c r="M282" t="n">
+        <v>16801</v>
+      </c>
+      <c r="N282" t="inlineStr">
+        <is>
+          <t>Tanaka Rie</t>
+        </is>
+      </c>
+      <c r="O282" t="inlineStr">
+        <is>
+          <t>Wada Arco</t>
+        </is>
+      </c>
+      <c r="P282" t="inlineStr">
+        <is>
+          <t>Earth</t>
+        </is>
+      </c>
+      <c r="Q282" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="R282" t="n">
+        <v>50</v>
+      </c>
+      <c r="S282" t="inlineStr">
+        <is>
+          <t>14.8%</t>
+        </is>
+      </c>
+      <c r="T282" t="inlineStr">
+        <is>
+          <t>0.6%</t>
+        </is>
+      </c>
+      <c r="U282" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="V282" t="inlineStr">
+        <is>
+          <t>0.5%</t>
+        </is>
+      </c>
+      <c r="W282" t="inlineStr">
+        <is>
+          <t>Lawful Evil</t>
+        </is>
+      </c>
+      <c r="X282" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y282" t="inlineStr">
+        <is>
+          <t>Female, Humanoid, Servant, Weak to Enuma Elish</t>
+        </is>
+      </c>
+      <c r="Z282" t="inlineStr">
+        <is>
+          <t>QAABB</t>
+        </is>
+      </c>
+      <c r="AA282" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB282" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC282" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD282" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE282" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AF282" t="inlineStr">
+        <is>
+          <t>Anti-World</t>
+        </is>
+      </c>
+      <c r="AG282" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="AH282" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Illyasviel von Einzbern (Archer)</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>286</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>4-Star</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Archer</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>イリヤスフィール・フォン・アインツベルン</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Illya</t>
+        </is>
+      </c>
+      <c r="G283" t="n">
+        <v>12</v>
+      </c>
+      <c r="H283" t="n">
+        <v>1683</v>
+      </c>
+      <c r="I283" t="n">
+        <v>10098</v>
+      </c>
+      <c r="J283" t="n">
+        <v>1746</v>
+      </c>
+      <c r="K283" t="n">
+        <v>10914</v>
+      </c>
+      <c r="L283" t="n">
+        <v>12226</v>
+      </c>
+      <c r="M283" t="n">
+        <v>13233</v>
+      </c>
+      <c r="N283" t="inlineStr">
+        <is>
+          <t>Kadowaki Mai, Takano Naoko</t>
+        </is>
+      </c>
+      <c r="O283" t="inlineStr">
+        <is>
+          <t>Hiroyama Hiroshi</t>
+        </is>
+      </c>
+      <c r="P283" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="Q283" t="inlineStr">
+        <is>
+          <t>Semi Reverse S</t>
+        </is>
+      </c>
+      <c r="R283" t="n">
+        <v>148</v>
+      </c>
+      <c r="S283" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
+      <c r="T283" t="inlineStr">
+        <is>
+          <t>0.63%</t>
+        </is>
+      </c>
+      <c r="U283" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="V283" t="inlineStr">
+        <is>
+          <t>31.5%</t>
+        </is>
+      </c>
+      <c r="W283" t="inlineStr">
+        <is>
+          <t>Neutral Summer</t>
+        </is>
+      </c>
+      <c r="X283" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y283" t="inlineStr">
+        <is>
+          <t>Children Servants, Female, Humanoid, Illya, Living Human, Pseudo-Servants, Servant, Weak to Enuma Elish</t>
+        </is>
+      </c>
+      <c r="Z283" t="inlineStr">
+        <is>
+          <t>QQAAB</t>
+        </is>
+      </c>
+      <c r="AA283" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB283" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC283" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD283" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE283" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AF283" t="inlineStr">
+        <is>
+          <t>Anti-Army</t>
+        </is>
+      </c>
+      <c r="AG283" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="AH283" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Brynhildr (Berserker)</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>287</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>4-Star</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Berserker</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>ブリュンヒルデ</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Brynhild (Brünnhilde), Sigrdrífa</t>
+        </is>
+      </c>
+      <c r="G284" t="n">
+        <v>12</v>
+      </c>
+      <c r="H284" t="n">
+        <v>1699</v>
+      </c>
+      <c r="I284" t="n">
+        <v>10197</v>
+      </c>
+      <c r="J284" t="n">
+        <v>1603</v>
+      </c>
+      <c r="K284" t="n">
+        <v>10023</v>
+      </c>
+      <c r="L284" t="n">
+        <v>12346</v>
+      </c>
+      <c r="M284" t="n">
+        <v>12153</v>
+      </c>
+      <c r="N284" t="inlineStr">
+        <is>
+          <t>Noto Mamiko</t>
+        </is>
+      </c>
+      <c r="O284" t="inlineStr">
+        <is>
+          <t>Miwa Shirō</t>
+        </is>
+      </c>
+      <c r="P284" t="inlineStr">
+        <is>
+          <t>Sky</t>
+        </is>
+      </c>
+      <c r="Q284" t="inlineStr">
+        <is>
+          <t>Semi Reverse S</t>
+        </is>
+      </c>
+      <c r="R284" t="n">
+        <v>10</v>
+      </c>
+      <c r="S284" t="inlineStr">
+        <is>
+          <t>5.1%</t>
+        </is>
+      </c>
+      <c r="T284" t="inlineStr">
+        <is>
+          <t>0.85%</t>
+        </is>
+      </c>
+      <c r="U284" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="V284" t="inlineStr">
+        <is>
+          <t>45.5%</t>
+        </is>
+      </c>
+      <c r="W284" t="inlineStr">
+        <is>
+          <t>Neutral Good</t>
+        </is>
+      </c>
+      <c r="X284" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y284" t="inlineStr">
+        <is>
+          <t>Divine, Female, Humanoid, Servant, Weak to Enuma Elish</t>
+        </is>
+      </c>
+      <c r="Z284" t="inlineStr">
+        <is>
+          <t>QABBB</t>
+        </is>
+      </c>
+      <c r="AA284" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB284" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC284" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD284" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE284" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AF284" t="inlineStr">
+        <is>
+          <t>Anti-Unit / Anti-Army</t>
+        </is>
+      </c>
+      <c r="AG284" t="inlineStr">
+        <is>
+          <t>Buster</t>
+        </is>
+      </c>
+      <c r="AH284" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Consort Yu (Lancer)</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>288</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>4-Star</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Lancer</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>虞美人</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Yu Miaoyi, Yu the Beauty, Yu Meiren, Akuta Hinako (芥ヒナコ?)Crimson Beauty Under the Moon (紅の月下美人?), Gubijin, Gucchan, 虞妙弋</t>
+        </is>
+      </c>
+      <c r="G285" t="n">
+        <v>12</v>
+      </c>
+      <c r="H285" t="n">
+        <v>1649</v>
+      </c>
+      <c r="I285" t="n">
+        <v>9896</v>
+      </c>
+      <c r="J285" t="n">
+        <v>1799</v>
+      </c>
+      <c r="K285" t="n">
+        <v>11245</v>
+      </c>
+      <c r="L285" t="n">
+        <v>11982</v>
+      </c>
+      <c r="M285" t="n">
+        <v>13634</v>
+      </c>
+      <c r="N285" t="inlineStr">
+        <is>
+          <t>Ise Mariya</t>
+        </is>
+      </c>
+      <c r="O285" t="inlineStr">
+        <is>
+          <t>toi8</t>
+        </is>
+      </c>
+      <c r="P285" t="inlineStr">
+        <is>
+          <t>Earth</t>
+        </is>
+      </c>
+      <c r="Q285" t="inlineStr">
+        <is>
+          <t>Reverse S</t>
+        </is>
+      </c>
+      <c r="R285" t="n">
+        <v>89</v>
+      </c>
+      <c r="S285" t="inlineStr">
+        <is>
+          <t>12.2%</t>
+        </is>
+      </c>
+      <c r="T285" t="inlineStr">
+        <is>
+          <t>1.1%</t>
+        </is>
+      </c>
+      <c r="U285" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="V285" t="inlineStr">
+        <is>
+          <t>24%</t>
+        </is>
+      </c>
+      <c r="W285" t="inlineStr">
+        <is>
+          <t>Lawful Evil</t>
+        </is>
+      </c>
+      <c r="X285" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y285" t="inlineStr">
+        <is>
+          <t>Demonic, Humanoid, Female, Servant, Weak to Enuma Elish</t>
+        </is>
+      </c>
+      <c r="Z285" t="inlineStr">
+        <is>
+          <t>QQABB</t>
+        </is>
+      </c>
+      <c r="AA285" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB285" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC285" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD285" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE285" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AF285" t="inlineStr">
+        <is>
+          <t>Anti-Army</t>
+        </is>
+      </c>
+      <c r="AG285" t="inlineStr">
+        <is>
+          <t>Quick</t>
+        </is>
+      </c>
+      <c r="AH285" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Abigail Williams (Summer)</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>289</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>5-Star</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Foreigner</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>アビゲイル・ウィリアムズ</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>The Key to the Gate, Sut-Typhon, Yog-Sothoth, All-in-One, One-in-All, Abby</t>
+        </is>
+      </c>
+      <c r="G286" t="n">
+        <v>16</v>
+      </c>
+      <c r="H286" t="n">
+        <v>1820</v>
+      </c>
+      <c r="I286" t="n">
+        <v>11781</v>
+      </c>
+      <c r="J286" t="n">
+        <v>2090</v>
+      </c>
+      <c r="K286" t="n">
+        <v>14250</v>
+      </c>
+      <c r="L286" t="n">
+        <v>12896</v>
+      </c>
+      <c r="M286" t="n">
+        <v>15611</v>
+      </c>
+      <c r="N286" t="inlineStr">
+        <is>
+          <t>Ōwada Hitomi</t>
+        </is>
+      </c>
+      <c r="O286" t="inlineStr">
+        <is>
+          <t>Kuroboshi Kouhaku</t>
+        </is>
+      </c>
+      <c r="P286" t="inlineStr">
+        <is>
+          <t>Earth</t>
+        </is>
+      </c>
+      <c r="Q286" t="inlineStr">
+        <is>
+          <t>Semi S</t>
+        </is>
+      </c>
+      <c r="R286" t="n">
+        <v>150</v>
+      </c>
+      <c r="S286" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="T286" t="inlineStr">
+        <is>
+          <t>0.86%</t>
+        </is>
+      </c>
+      <c r="U286" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="V286" t="inlineStr">
+        <is>
+          <t>6%</t>
+        </is>
+      </c>
+      <c r="W286" t="inlineStr">
+        <is>
+          <t>Lawful Evil</t>
+        </is>
+      </c>
+      <c r="X286" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y286" t="inlineStr">
+        <is>
+          <t>Children Servants, Divine, Female, Humanoid, Servant, Threat to Humanity</t>
+        </is>
+      </c>
+      <c r="Z286" t="inlineStr">
+        <is>
+          <t>QQABB</t>
+        </is>
+      </c>
+      <c r="AA286" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB286" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC286" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD286" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE286" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AF286" t="inlineStr">
+        <is>
+          <t>Anti-Unit</t>
+        </is>
+      </c>
+      <c r="AG286" t="inlineStr">
+        <is>
+          <t>Buster</t>
+        </is>
+      </c>
+      <c r="AH286" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Tomoe Gozen (Saber)</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>290</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>4-Star</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Saber</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>巴御前</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G287" t="n">
+        <v>12</v>
+      </c>
+      <c r="H287" t="n">
+        <v>1590</v>
+      </c>
+      <c r="I287" t="n">
+        <v>9544</v>
+      </c>
+      <c r="J287" t="n">
+        <v>1957</v>
+      </c>
+      <c r="K287" t="n">
+        <v>12233</v>
+      </c>
+      <c r="L287" t="n">
+        <v>11556</v>
+      </c>
+      <c r="M287" t="n">
+        <v>14832</v>
+      </c>
+      <c r="N287" t="inlineStr">
+        <is>
+          <t>Kanemoto Hisako</t>
+        </is>
+      </c>
+      <c r="O287" t="inlineStr">
+        <is>
+          <t>Shirabi</t>
+        </is>
+      </c>
+      <c r="P287" t="inlineStr">
+        <is>
+          <t>Earth</t>
+        </is>
+      </c>
+      <c r="Q287" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="R287" t="n">
+        <v>102</v>
+      </c>
+      <c r="S287" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+      <c r="T287" t="inlineStr">
+        <is>
+          <t>0.55%</t>
+        </is>
+      </c>
+      <c r="U287" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="V287" t="inlineStr">
+        <is>
+          <t>24.5%</t>
+        </is>
+      </c>
+      <c r="W287" t="inlineStr">
+        <is>
+          <t>Neutral   Good</t>
+        </is>
+      </c>
+      <c r="X287" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="Y287" t="inlineStr">
+        <is>
+          <t>Demonic, Female, Humanoid, Riding, Servant, Weak to Enuma Elish</t>
+        </is>
+      </c>
+      <c r="Z287" t="inlineStr">
+        <is>
+          <t>QAABB</t>
+        </is>
+      </c>
+      <c r="AA287" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB287" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC287" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD287" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE287" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AF287" t="inlineStr">
+        <is>
+          <t>Anti-Army</t>
+        </is>
+      </c>
+      <c r="AG287" t="inlineStr">
+        <is>
+          <t>Arts</t>
+        </is>
+      </c>
+      <c r="AH287" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>